<commit_message>
v4.0 - Zmiana do przedstawienia projektu
</commit_message>
<xml_diff>
--- a/Projekt2/Sortowanie.xlsx
+++ b/Projekt2/Sortowanie.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piotr\source\repos\Piotr601\PAMSI\Projekt2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364BA66C-F08E-4F19-9DF3-FEF411193F38}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C34195B-2A09-467B-8038-A32B9E0583F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EBD6B448-DD81-4078-9D8E-CABD40A131B1}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -187,11 +187,12 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -199,12 +200,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6661,8 +6661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C10C85-ABC6-48C6-80D6-99015EA13158}">
   <dimension ref="B3:O97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H51" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="V56" sqref="V56"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V43" sqref="V43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6673,54 +6673,54 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="I3" s="17" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="I3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
-      <c r="C4" s="20">
+      <c r="C4" s="16">
         <v>10000</v>
       </c>
-      <c r="D4" s="20">
+      <c r="D4" s="16">
         <v>50000</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="16">
         <v>100000</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="16">
         <v>500000</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="16">
         <v>1000000</v>
       </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="20">
+      <c r="J4" s="16">
         <v>10000</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="16">
         <v>50000</v>
       </c>
-      <c r="L4" s="20">
+      <c r="L4" s="16">
         <v>100000</v>
       </c>
-      <c r="M4" s="20">
+      <c r="M4" s="16">
         <v>500000</v>
       </c>
-      <c r="N4" s="20">
+      <c r="N4" s="16">
         <v>1000000</v>
       </c>
     </row>
@@ -6796,10 +6796,10 @@
       <c r="M6" s="7">
         <v>0.66742000000000001</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="18">
         <v>1.3827</v>
       </c>
-      <c r="O6" s="21"/>
+      <c r="O6" s="17"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
@@ -7031,54 +7031,54 @@
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="I15" s="19" t="s">
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="I15" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
-      <c r="C16" s="20">
+      <c r="C16" s="16">
         <v>10000</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="16">
         <v>50000</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="16">
         <v>100000</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="16">
         <v>500000</v>
       </c>
-      <c r="G16" s="20">
+      <c r="G16" s="16">
         <v>1000000</v>
       </c>
       <c r="I16" s="1"/>
-      <c r="J16" s="20">
+      <c r="J16" s="16">
         <v>10000</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16" s="16">
         <v>50000</v>
       </c>
-      <c r="L16" s="20">
+      <c r="L16" s="16">
         <v>100000</v>
       </c>
-      <c r="M16" s="20">
+      <c r="M16" s="16">
         <v>500000</v>
       </c>
-      <c r="N16" s="20">
+      <c r="N16" s="16">
         <v>1000000</v>
       </c>
     </row>
@@ -7387,54 +7387,54 @@
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C76" s="16"/>
-      <c r="D76" s="16"/>
-      <c r="E76" s="16"/>
-      <c r="F76" s="16"/>
-      <c r="G76" s="16"/>
-      <c r="I76" s="17" t="s">
+      <c r="C76" s="21"/>
+      <c r="D76" s="21"/>
+      <c r="E76" s="21"/>
+      <c r="F76" s="21"/>
+      <c r="G76" s="21"/>
+      <c r="I76" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="J76" s="17"/>
-      <c r="K76" s="17"/>
-      <c r="L76" s="17"/>
-      <c r="M76" s="17"/>
-      <c r="N76" s="17"/>
+      <c r="J76" s="22"/>
+      <c r="K76" s="22"/>
+      <c r="L76" s="22"/>
+      <c r="M76" s="22"/>
+      <c r="N76" s="22"/>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B77" s="1"/>
-      <c r="C77" s="20">
+      <c r="C77" s="16">
         <v>10000</v>
       </c>
-      <c r="D77" s="20">
+      <c r="D77" s="16">
         <v>50000</v>
       </c>
-      <c r="E77" s="20">
+      <c r="E77" s="16">
         <v>100000</v>
       </c>
-      <c r="F77" s="20">
+      <c r="F77" s="16">
         <v>500000</v>
       </c>
-      <c r="G77" s="20">
+      <c r="G77" s="16">
         <v>1000000</v>
       </c>
       <c r="I77" s="1"/>
-      <c r="J77" s="20">
+      <c r="J77" s="16">
         <v>10000</v>
       </c>
-      <c r="K77" s="20">
+      <c r="K77" s="16">
         <v>50000</v>
       </c>
-      <c r="L77" s="20">
+      <c r="L77" s="16">
         <v>100000</v>
       </c>
-      <c r="M77" s="20">
+      <c r="M77" s="16">
         <v>500000</v>
       </c>
-      <c r="N77" s="20">
+      <c r="N77" s="16">
         <v>1000000</v>
       </c>
     </row>
@@ -7743,54 +7743,54 @@
       </c>
     </row>
     <row r="88" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C88" s="18"/>
-      <c r="D88" s="18"/>
-      <c r="E88" s="18"/>
-      <c r="F88" s="18"/>
-      <c r="G88" s="18"/>
-      <c r="I88" s="19" t="s">
+      <c r="C88" s="19"/>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="G88" s="19"/>
+      <c r="I88" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="J88" s="19"/>
-      <c r="K88" s="19"/>
-      <c r="L88" s="19"/>
-      <c r="M88" s="19"/>
-      <c r="N88" s="19"/>
+      <c r="J88" s="20"/>
+      <c r="K88" s="20"/>
+      <c r="L88" s="20"/>
+      <c r="M88" s="20"/>
+      <c r="N88" s="20"/>
     </row>
     <row r="89" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B89" s="1"/>
-      <c r="C89" s="20">
+      <c r="C89" s="16">
         <v>10000</v>
       </c>
-      <c r="D89" s="20">
+      <c r="D89" s="16">
         <v>50000</v>
       </c>
-      <c r="E89" s="20">
+      <c r="E89" s="16">
         <v>100000</v>
       </c>
-      <c r="F89" s="20">
+      <c r="F89" s="16">
         <v>500000</v>
       </c>
-      <c r="G89" s="20">
+      <c r="G89" s="16">
         <v>1000000</v>
       </c>
       <c r="I89" s="1"/>
-      <c r="J89" s="20">
+      <c r="J89" s="16">
         <v>10000</v>
       </c>
-      <c r="K89" s="20">
+      <c r="K89" s="16">
         <v>50000</v>
       </c>
-      <c r="L89" s="20">
+      <c r="L89" s="16">
         <v>100000</v>
       </c>
-      <c r="M89" s="20">
+      <c r="M89" s="16">
         <v>500000</v>
       </c>
-      <c r="N89" s="20">
+      <c r="N89" s="16">
         <v>1000000</v>
       </c>
     </row>

</xml_diff>